<commit_message>
updating temperature sensor part list & software
</commit_message>
<xml_diff>
--- a/Hardware/KiCAD/TemperatureSensor/DigiKey-PartsList.xlsx
+++ b/Hardware/KiCAD/TemperatureSensor/DigiKey-PartsList.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daniel\Dropbox (MIT)\Projects\IsoDAR\Ion Source\Control System\Hardware\KiCAD\TemperatureSensor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Dropbox\Work\conrad\isodar\Ion-Source-Control-System\Hardware\KiCAD\TemperatureSensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8052" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="First Order" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
   <si>
     <t>name</t>
   </si>
@@ -121,6 +121,15 @@
   </si>
   <si>
     <t>MAX31856MUD+-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CP-048H-ND </t>
+  </si>
+  <si>
+    <t>486-2019-ND</t>
+  </si>
+  <si>
+    <t>BZT52C15S-FDICT-ND</t>
   </si>
 </sst>
 </file>
@@ -492,16 +501,16 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,7 +521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -523,7 +532,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -534,7 +543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -545,7 +554,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -556,7 +565,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -567,7 +576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -578,7 +587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -589,7 +598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -600,7 +609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -611,7 +620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -622,7 +631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -633,7 +642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -655,17 +664,17 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -676,7 +685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -687,7 +696,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -698,7 +707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -709,7 +718,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -720,40 +729,40 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
+      <c r="B6" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
-        <v>20</v>
+      <c r="B8" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -764,7 +773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -775,7 +784,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -786,7 +795,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -797,7 +806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -808,7 +817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
updated parts list with arduino-compatible barrel jack
</commit_message>
<xml_diff>
--- a/Hardware/KiCAD/TemperatureSensor/DigiKey-PartsList.xlsx
+++ b/Hardware/KiCAD/TemperatureSensor/DigiKey-PartsList.xlsx
@@ -123,13 +123,13 @@
     <t>MAX31856MUD+-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">CP-048H-ND </t>
-  </si>
-  <si>
     <t>486-2019-ND</t>
   </si>
   <si>
     <t>BZT52C15S-FDICT-ND</t>
+  </si>
+  <si>
+    <t>CP-202AH-ND</t>
   </si>
 </sst>
 </file>
@@ -664,7 +664,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -734,7 +734,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -745,7 +745,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="2">
         <v>2</v>
@@ -756,7 +756,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>

</xml_diff>